<commit_message>
work on battle logic
</commit_message>
<xml_diff>
--- a/manage/battleAlgorytmus.xlsx
+++ b/manage/battleAlgorytmus.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.buryan\Documents\x_other\2D_js\DigitalDungen\manage\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF4B41A-B9A7-4FDE-ABA0-2E84D1F4892E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="30" windowWidth="13380" windowHeight="5840"/>
+    <workbookView xWindow="315" yWindow="30" windowWidth="13380" windowHeight="5835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
   <si>
     <t>hero</t>
   </si>
@@ -48,9 +54,6 @@
     <t>Monster attacks</t>
   </si>
   <si>
-    <t>potential dmg</t>
-  </si>
-  <si>
     <t>moster.strength</t>
   </si>
   <si>
@@ -60,14 +63,68 @@
     <t>moster.strength * missDiceRoll</t>
   </si>
   <si>
-    <t>missDiceRoll = random number 0 to 9 - if (0 to 3) {attack missed} - if ( 4 to 5) {attack potential 50 to 60 %} -</t>
+    <t xml:space="preserve">missDiceRoll = random number 0 to 9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">// if (0 to 3) {attack missed} 
+// if ( 4 to 5) {attack potential 50 to 70 %} 
+// if ( 6 to 7) {attack potential 71 to 90 %} 
+// if ( 8 to 9) { attack potential 91 to 100 % } </t>
+  </si>
+  <si>
+    <t>monster potential dmg</t>
+  </si>
+  <si>
+    <t>potential hero dmg</t>
+  </si>
+  <si>
+    <t>hero receives damage</t>
+  </si>
+  <si>
+    <t>2)</t>
+  </si>
+  <si>
+    <t>hero deffence</t>
+  </si>
+  <si>
+    <t>hero.defense + hero.armor.head + hero.armor.shield + hero.armor.chestPlate + hero.armor.shoes</t>
+  </si>
+  <si>
+    <t>hero received dmg = actual moster attack - hero deffence</t>
+  </si>
+  <si>
+    <t>armor damage = 10%</t>
+  </si>
+  <si>
+    <t>hero.strength + hero.weapon.power + hero.spell.chanted</t>
+  </si>
+  <si>
+    <t>actual hero attack</t>
+  </si>
+  <si>
+    <t>potential hero dmg * missDiceRoll</t>
+  </si>
+  <si>
+    <t>3)</t>
+  </si>
+  <si>
+    <t>monster receives gamage</t>
+  </si>
+  <si>
+    <t>hero attacks</t>
+  </si>
+  <si>
+    <t>IF hero health is 0 or lower</t>
+  </si>
+  <si>
+    <t>HERO DIES, GAME ENDS (show game results)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,18 +141,42 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Consolas"/>
       <family val="3"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,10 +191,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -124,14 +211,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
-    <a:clrScheme name="Kancelář">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,9 +259,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kancelář">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -204,9 +294,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,9 +346,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kancelář">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -414,25 +538,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7265625" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -440,7 +566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -457,7 +583,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -474,7 +600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
@@ -491,7 +617,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -508,36 +634,105 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:9" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
         <v>10</v>
       </c>
-      <c r="C15" t="s">
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="C17" t="s">
-        <v>13</v>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -547,24 +742,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
corrected hero attack path
</commit_message>
<xml_diff>
--- a/manage/battleAlgorytmus.xlsx
+++ b/manage/battleAlgorytmus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.buryan\Documents\x_other\2D_js\DigitalDungen\manage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF4B41A-B9A7-4FDE-ABA0-2E84D1F4892E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F76D28-48CB-4BFF-B56A-8087007E64D1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="30" windowWidth="13380" windowHeight="5835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>hero</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>strength;</t>
-  </si>
-  <si>
-    <t>defense;</t>
   </si>
   <si>
     <t>hitPoints = 100;</t>
@@ -87,9 +84,6 @@
     <t>hero deffence</t>
   </si>
   <si>
-    <t>hero.defense + hero.armor.head + hero.armor.shield + hero.armor.chestPlate + hero.armor.shoes</t>
-  </si>
-  <si>
     <t>hero received dmg = actual moster attack - hero deffence</t>
   </si>
   <si>
@@ -118,6 +112,33 @@
   </si>
   <si>
     <t>HERO DIES, GAME ENDS (show game results)</t>
+  </si>
+  <si>
+    <t>if "hero deffence" &lt; "actual monster attack"</t>
+  </si>
+  <si>
+    <t>monster deffence</t>
+  </si>
+  <si>
+    <t>monster.deffence</t>
+  </si>
+  <si>
+    <t>monster received dmg = actual hero attack - monster deffence</t>
+  </si>
+  <si>
+    <t>4)</t>
+  </si>
+  <si>
+    <t>hero chooses defence</t>
+  </si>
+  <si>
+    <t>if "actual hero attack" &lt; "monster defence"</t>
+  </si>
+  <si>
+    <t>defence;</t>
+  </si>
+  <si>
+    <t>hero.defence + hero.armor.head + hero.armor.shield + hero.armor.chestPlate + hero.armor.shoes</t>
   </si>
 </sst>
 </file>
@@ -539,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I35"/>
+  <dimension ref="B1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,12 +574,12 @@
     <col min="8" max="8" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -566,7 +587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -583,15 +604,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -600,15 +621,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>100</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H7">
         <v>100</v>
@@ -617,15 +638,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -634,105 +655,131 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="5" t="s">
+    </row>
+    <row r="15" spans="2:13" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
       <c r="G15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
         <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>30</v>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C31" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>27</v>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added hero defends algorytm
</commit_message>
<xml_diff>
--- a/manage/battleAlgorytmus.xlsx
+++ b/manage/battleAlgorytmus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.buryan\Documents\x_other\2D_js\DigitalDungen\manage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F76D28-48CB-4BFF-B56A-8087007E64D1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71705D44-7789-48A2-9ED5-2B5C27A0B78A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="30" windowWidth="13380" windowHeight="5835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>hero</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>hero.defence + hero.armor.head + hero.armor.shield + hero.armor.chestPlate + hero.armor.shoes</t>
+  </si>
+  <si>
+    <t>armor damage = 5%</t>
+  </si>
+  <si>
+    <t>hero.defence + ( hero.strength + 50%) + hero.armor.head + hero.armor.shield + hero.armor.chestPlate + hero.armor.shoes</t>
   </si>
 </sst>
 </file>
@@ -560,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M43"/>
+  <dimension ref="B1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,14 +578,16 @@
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="13" max="13" width="22.85546875" customWidth="1"/>
+    <col min="19" max="19" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -587,7 +595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -604,7 +612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
@@ -621,7 +629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -638,7 +646,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -655,7 +663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
@@ -663,15 +671,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="2:13" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -684,55 +698,100 @@
       <c r="H15" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="M17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="M19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="N26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="M29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
         <v>24</v>
       </c>

</xml_diff>